<commit_message>
Added code and table for population data
</commit_message>
<xml_diff>
--- a/Data/Vinmonopolet/Kommune_data_final.xlsx
+++ b/Data/Vinmonopolet/Kommune_data_final.xlsx
@@ -541,7 +541,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Våler</t>
+          <t>Våler (Østfold)</t>
         </is>
       </c>
       <c r="C8">
@@ -589,7 +589,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Indre</t>
+          <t>Indre Østfold</t>
         </is>
       </c>
       <c r="C10">
@@ -757,7 +757,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Nordre</t>
+          <t>Nordre Follo</t>
         </is>
       </c>
       <c r="C17">
@@ -1333,7 +1333,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Øvre</t>
+          <t>Øvre Eiker</t>
         </is>
       </c>
       <c r="C41">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Nore</t>
+          <t>Nore og Uvdal</t>
         </is>
       </c>
       <c r="C53">
@@ -1933,7 +1933,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Våler</t>
+          <t>Våler (Innlandet)</t>
         </is>
       </c>
       <c r="C66">
@@ -2485,7 +2485,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Østre</t>
+          <t>Østre Toten</t>
         </is>
       </c>
       <c r="C89">
@@ -2509,7 +2509,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Vestre</t>
+          <t>Vestre Toten</t>
         </is>
       </c>
       <c r="C90">
@@ -2557,7 +2557,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Søndre</t>
+          <t>Søndre Land</t>
         </is>
       </c>
       <c r="C92">
@@ -2581,7 +2581,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Nordre</t>
+          <t>Nordre Land</t>
         </is>
       </c>
       <c r="C93">
@@ -2677,7 +2677,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Vestre</t>
+          <t>Vestre Slidre</t>
         </is>
       </c>
       <c r="C97">
@@ -2701,7 +2701,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Øystre</t>
+          <t>Øystre Slidre</t>
         </is>
       </c>
       <c r="C98">
@@ -3661,7 +3661,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Evje</t>
+          <t>Evje og Hornnes</t>
         </is>
       </c>
       <c r="C138">
@@ -5605,7 +5605,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Herøy</t>
+          <t>Herøy (Møre og Romsdal)</t>
         </is>
       </c>
       <c r="C219">
@@ -6133,7 +6133,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Trondheim</t>
+          <t>Trondheim - Tråante</t>
         </is>
       </c>
       <c r="C241">
@@ -6181,7 +6181,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Namsos</t>
+          <t>Namsos - Nåavmesjenjaelmie</t>
         </is>
       </c>
       <c r="C243">
@@ -6301,7 +6301,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Røros</t>
+          <t>Røros - Rosse</t>
         </is>
       </c>
       <c r="C248">
@@ -6349,7 +6349,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Midtre</t>
+          <t>Midtre Gauldal</t>
         </is>
       </c>
       <c r="C250">
@@ -6565,7 +6565,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Levanger</t>
+          <t>Levanger - Levangke</t>
         </is>
       </c>
       <c r="C259">
@@ -6613,7 +6613,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Snåase</t>
+          <t>Snåase - Snåsa</t>
         </is>
       </c>
       <c r="C261">
@@ -6661,7 +6661,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Raarvihke</t>
+          <t>Raarvihke - Røyrvik</t>
         </is>
       </c>
       <c r="C263">
@@ -6853,7 +6853,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Indre</t>
+          <t>Indre Fosen</t>
         </is>
       </c>
       <c r="C271">
@@ -7213,7 +7213,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Herøy</t>
+          <t>Herøy (Nordland)</t>
         </is>
       </c>
       <c r="C286">
@@ -7333,7 +7333,7 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Aarborte</t>
+          <t>Aarborte - Hattfjelldal</t>
         </is>
       </c>
       <c r="C291">
@@ -7429,7 +7429,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Rana</t>
+          <t>Rana - Raane</t>
         </is>
       </c>
       <c r="C295">
@@ -7621,7 +7621,7 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Fauske</t>
+          <t>Fauske - Fuossko</t>
         </is>
       </c>
       <c r="C303">
@@ -7645,7 +7645,7 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Sørfold</t>
+          <t>Sørfold - Fuolldá</t>
         </is>
       </c>
       <c r="C304">
@@ -7717,7 +7717,7 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Evenes</t>
+          <t>Evenes - Evenássi</t>
         </is>
       </c>
       <c r="C307">
@@ -7885,7 +7885,7 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Bø</t>
+          <t>Bø (Nordland)</t>
         </is>
       </c>
       <c r="C314">
@@ -7933,7 +7933,7 @@
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Sortland</t>
+          <t>Sortland - Suortá</t>
         </is>
       </c>
       <c r="C316">
@@ -8005,7 +8005,7 @@
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Hábmer</t>
+          <t>Hábmer - Hamarøy</t>
         </is>
       </c>
       <c r="C319">
@@ -8053,7 +8053,7 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Harstad</t>
+          <t>Harstad - Hárstták</t>
         </is>
       </c>
       <c r="C321">
@@ -8101,7 +8101,7 @@
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Dielddanuorri</t>
+          <t>Dielddanuorri - Tjeldsund</t>
         </is>
       </c>
       <c r="C323">
@@ -8149,7 +8149,7 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>Gratangen</t>
+          <t>Gratangen - Rivtták</t>
         </is>
       </c>
       <c r="C325">
@@ -8173,7 +8173,7 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Loabák</t>
+          <t>Loabák - Lavangen</t>
         </is>
       </c>
       <c r="C326">
@@ -8413,7 +8413,7 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>Storfjord</t>
+          <t>Storfjord - Omasvuotna - Omasvuono</t>
         </is>
       </c>
       <c r="C336">
@@ -8437,7 +8437,7 @@
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>Gáivuotna</t>
+          <t>Gáivuotna - Kåfjord - Kaivuono</t>
         </is>
       </c>
       <c r="C337">
@@ -8485,7 +8485,7 @@
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>Nordreisa</t>
+          <t>Nordreisa - Ráisa - Raisi</t>
         </is>
       </c>
       <c r="C339">
@@ -8557,7 +8557,7 @@
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>Hammerfest</t>
+          <t>Hammerfest - Hámmerfeasta</t>
         </is>
       </c>
       <c r="C342">
@@ -8629,7 +8629,7 @@
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>Kárásjohka</t>
+          <t>Kárásjohka - Karasjok</t>
         </is>
       </c>
       <c r="C345">
@@ -8653,7 +8653,7 @@
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>Guovdageaidnu</t>
+          <t>Guovdageaidnu - Kautokeino</t>
         </is>
       </c>
       <c r="C346">
@@ -8773,7 +8773,7 @@
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>Porsanger</t>
+          <t>Porsanger - Porsángu - Porsanki</t>
         </is>
       </c>
       <c r="C351">
@@ -8845,7 +8845,7 @@
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>Deatnu</t>
+          <t>Deatnu - Tana</t>
         </is>
       </c>
       <c r="C354">
@@ -8941,7 +8941,7 @@
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>Unjárga</t>
+          <t>Unjárga - Nesseby</t>
         </is>
       </c>
       <c r="C358">

</xml_diff>